<commit_message>
excel upload for specials to accomodate new field
</commit_message>
<xml_diff>
--- a/backend/explore/sample.xlsx
+++ b/backend/explore/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzobule\Documents\flysolomons\website\backend\explore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4D4CA2-E954-402D-BACC-04426DE424F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9586FD0-FD51-4AC7-BCA8-CD0D37C29AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Special ID</t>
   </si>
@@ -42,10 +42,16 @@
     <t>EARLY-2025</t>
   </si>
   <si>
-    <t>HIR-BNE</t>
-  </si>
-  <si>
     <t>Return</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>HIR-AKL</t>
   </si>
 </sst>
 </file>
@@ -363,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,7 +382,7 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -389,19 +395,25 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>1000</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>